<commit_message>
fdr_worksheet works. Fields ready for validating
</commit_message>
<xml_diff>
--- a/tests/unit/fdr_simple.xlsx
+++ b/tests/unit/fdr_simple.xlsx
@@ -1,23 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chuki\projects\fdr\tests\unit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchukina\projects\fdr\tests\unit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B1F942-0430-4612-B1C3-F6EC78F65C6C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB3AC63-7689-44F2-97DB-D7FD23EC5F4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="import_worksheet" sheetId="21" r:id="rId1"/>
+    <sheet name="Procedure Based Requirements" sheetId="22" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">import_worksheet!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Procedure Based Requirements'!$A$1:$O$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">import_worksheet!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Procedure Based Requirements'!$1:$1</definedName>
+    <definedName name="rngRequirements" localSheetId="1">#REF!</definedName>
     <definedName name="rngRequirements">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -25,7 +29,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
@@ -647,8 +650,221 @@
   </sheetPr>
   <dimension ref="A1:O3"/>
   <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" style="3" customWidth="1"/>
+    <col min="2" max="7" width="4.7109375" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="21.85546875" customWidth="1"/>
+    <col min="9" max="9" width="61.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="33.42578125" customWidth="1"/>
+    <col min="11" max="11" width="32.140625" customWidth="1"/>
+    <col min="12" max="12" width="25.7109375" customWidth="1"/>
+    <col min="13" max="13" width="23.5703125" customWidth="1"/>
+    <col min="14" max="14" width="31.140625" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="87.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="str">
+        <f>_xlfn.CONCAT(A1, " value")</f>
+        <v>ID value</v>
+      </c>
+      <c r="B2" s="3" t="str">
+        <f t="shared" ref="B2:O3" si="0">_xlfn.CONCAT(B1, " value")</f>
+        <v>Procedure Step value</v>
+      </c>
+      <c r="C2" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>User Need value</v>
+      </c>
+      <c r="D2" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Design Input value</v>
+      </c>
+      <c r="E2" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>DO Solution L1 value</v>
+      </c>
+      <c r="F2" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>DO Solution L2 value</v>
+      </c>
+      <c r="G2" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>DO Solution L3 value</v>
+      </c>
+      <c r="H2" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Cascade Level value</v>
+      </c>
+      <c r="I2" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Requirement Statement value</v>
+      </c>
+      <c r="J2" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Requirement Rationale value</v>
+      </c>
+      <c r="K2" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Verification or
+Validation Strategy value</v>
+      </c>
+      <c r="L2" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Verification or Validation Results value</v>
+      </c>
+      <c r="M2" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Devices value</v>
+      </c>
+      <c r="N2" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Design Ouptut Feature
+(with CTQ ID #) value</v>
+      </c>
+      <c r="O2" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>CTQ?
+Yes, No, N/A value</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="str">
+        <f>_xlfn.CONCAT(A2, " value")</f>
+        <v>ID value value</v>
+      </c>
+      <c r="B3" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Procedure Step value value</v>
+      </c>
+      <c r="C3" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>User Need value value</v>
+      </c>
+      <c r="D3" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Design Input value value</v>
+      </c>
+      <c r="E3" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>DO Solution L1 value value</v>
+      </c>
+      <c r="F3" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>DO Solution L2 value value</v>
+      </c>
+      <c r="G3" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>DO Solution L3 value value</v>
+      </c>
+      <c r="H3" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Cascade Level value value</v>
+      </c>
+      <c r="I3" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Requirement Statement value value</v>
+      </c>
+      <c r="J3" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Requirement Rationale value value</v>
+      </c>
+      <c r="K3" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Verification or
+Validation Strategy value value</v>
+      </c>
+      <c r="L3" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Verification or Validation Results value value</v>
+      </c>
+      <c r="M3" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Devices value value</v>
+      </c>
+      <c r="N3" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Design Ouptut Feature
+(with CTQ ID #) value value</v>
+      </c>
+      <c r="O3" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>CTQ?
+Yes, No, N/A value value</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:O1" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="17" scale="71" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;CPage &amp;P of &amp;N&amp;RVersion 2.0</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52B51914-4951-4CB5-B02A-D6D464BC6724}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:O3"/>
+  <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -889,15 +1105,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004B2369C55104614D86A5ED6959977478" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c0e7eb4f9a047313f41567777b26d1b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e53f4f12-70f6-49ff-8342-256ad4d5af45" xmlns:ns3="4f4d318f-1e15-433d-b7fd-4a4fd8f11b5b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="21513b83e70fc08b789b5f083b414370" ns2:_="" ns3:_="">
     <xsd:import namespace="e53f4f12-70f6-49ff-8342-256ad4d5af45"/>
@@ -1176,6 +1383,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E6B224B-0E2C-48D8-BDA5-831DA84116C8}">
   <ds:schemaRefs>
@@ -1194,14 +1410,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0EA3E94-102E-42ED-8307-567DE6417681}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB17CD09-13F0-4BBC-ACF0-5247DAC323D1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1218,4 +1426,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0EA3E94-102E-42ED-8307-567DE6417681}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>